<commit_message>
Primer documento: Cronograma con titulo
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52646\Downloads\Proyecto BD Almacen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52646\Desktop\ProyectoBDITE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86DF7823-7935-4863-86E6-A3A411D2C207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096D605B-4BAF-4401-9DC4-6DCEC75F8EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77C97420-D882-4AEC-80C4-94E9F25F4DD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Marzo</t>
   </si>
@@ -128,13 +128,16 @@
   </si>
   <si>
     <t>Alimentar la BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRONOGRAMA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +203,14 @@
       <color theme="0"/>
       <name val="Arial Nova"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -624,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -636,32 +647,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,85 +660,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1070,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770ABD26-0474-45FB-9EFD-7F425FDDCB3A}">
-  <dimension ref="G2:AN29"/>
+  <dimension ref="G1:AN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,143 +1097,172 @@
     <col min="12" max="12" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="7:40" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="O1" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="58"/>
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="58"/>
+    </row>
     <row r="2" spans="7:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="7:40" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="7" t="s">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="14" t="s">
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="17" t="s">
+      <c r="AC3" s="52"/>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="52"/>
+      <c r="AI3" s="52"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AL3" s="17"/>
-      <c r="AM3" s="18"/>
+      <c r="AL3" s="54"/>
+      <c r="AM3" s="55"/>
     </row>
     <row r="4" spans="7:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I4" s="2"/>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30" t="s">
+      <c r="P4" s="57"/>
+      <c r="Q4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32" t="s">
+      <c r="R4" s="42"/>
+      <c r="S4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="30" t="s">
+      <c r="T4" s="45"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="30" t="s">
+      <c r="W4" s="44"/>
+      <c r="X4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="30" t="s">
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="34" t="s">
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="30" t="s">
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="30" t="s">
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="32"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="30" t="s">
+      <c r="AG4" s="45"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="32" t="s">
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="32"/>
-      <c r="AM4" s="31"/>
+      <c r="AL4" s="45"/>
+      <c r="AM4" s="42"/>
       <c r="AN4" s="4"/>
     </row>
     <row r="5" spans="7:40" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="35"/>
-      <c r="N5" s="19">
+      <c r="L5" s="36"/>
+      <c r="N5" s="12">
         <v>18</v>
       </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="22"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="21"/>
-      <c r="AM5" s="22"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="15"/>
       <c r="AN5" s="4"/>
     </row>
     <row r="6" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J6" s="36">
+      <c r="J6" s="18">
         <v>1</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="38"/>
+      <c r="L6" s="40"/>
       <c r="N6" s="5">
         <v>20</v>
       </c>
-      <c r="O6" s="9"/>
+      <c r="O6" s="7"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="10"/>
+      <c r="R6" s="8"/>
       <c r="S6" s="6"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -1229,7 +1272,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="9"/>
+      <c r="AB6" s="7"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
@@ -1237,31 +1280,31 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
-      <c r="AJ6" s="10"/>
+      <c r="AJ6" s="8"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="1"/>
-      <c r="AM6" s="10"/>
+      <c r="AM6" s="8"/>
       <c r="AN6" s="4"/>
     </row>
     <row r="7" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="J7" s="36">
+      <c r="H7" s="37"/>
+      <c r="J7" s="18">
         <v>2</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="38"/>
+      <c r="L7" s="40"/>
       <c r="N7" s="3">
         <v>25</v>
       </c>
-      <c r="O7" s="9"/>
+      <c r="O7" s="7"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="10"/>
+      <c r="R7" s="8"/>
       <c r="S7" s="6"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -1271,7 +1314,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="9"/>
+      <c r="AB7" s="7"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
@@ -1279,29 +1322,29 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
-      <c r="AJ7" s="10"/>
+      <c r="AJ7" s="8"/>
       <c r="AK7" s="6"/>
       <c r="AL7" s="1"/>
-      <c r="AM7" s="10"/>
+      <c r="AM7" s="8"/>
       <c r="AN7" s="4"/>
     </row>
     <row r="8" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="J8" s="36">
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="J8" s="18">
         <v>3</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="38"/>
+      <c r="L8" s="40"/>
       <c r="N8" s="5">
         <v>27</v>
       </c>
-      <c r="O8" s="9"/>
+      <c r="O8" s="7"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="10"/>
+      <c r="R8" s="8"/>
       <c r="S8" s="6"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -1311,7 +1354,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="9"/>
+      <c r="AB8" s="7"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
@@ -1319,33 +1362,33 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
-      <c r="AJ8" s="10"/>
+      <c r="AJ8" s="8"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="1"/>
-      <c r="AM8" s="10"/>
+      <c r="AM8" s="8"/>
       <c r="AN8" s="4"/>
     </row>
     <row r="9" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="36">
+      <c r="J9" s="18">
         <v>4</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="40"/>
+      <c r="L9" s="20"/>
       <c r="N9" s="3">
         <v>1</v>
       </c>
-      <c r="O9" s="9"/>
+      <c r="O9" s="7"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="10"/>
+      <c r="R9" s="8"/>
       <c r="S9" s="6"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1355,7 +1398,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="9"/>
+      <c r="AB9" s="7"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
@@ -1363,33 +1406,33 @@
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
-      <c r="AJ9" s="10"/>
+      <c r="AJ9" s="8"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="1"/>
-      <c r="AM9" s="10"/>
+      <c r="AM9" s="8"/>
       <c r="AN9" s="4"/>
     </row>
     <row r="10" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="18">
         <v>5</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="42"/>
+      <c r="L10" s="33"/>
       <c r="N10" s="5">
         <v>3</v>
       </c>
-      <c r="O10" s="9"/>
+      <c r="O10" s="7"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="10"/>
+      <c r="R10" s="8"/>
       <c r="S10" s="6"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1399,7 +1442,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="9"/>
+      <c r="AB10" s="7"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
@@ -1407,27 +1450,27 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
-      <c r="AJ10" s="10"/>
+      <c r="AJ10" s="8"/>
       <c r="AK10" s="6"/>
       <c r="AL10" s="1"/>
-      <c r="AM10" s="10"/>
+      <c r="AM10" s="8"/>
       <c r="AN10" s="4"/>
     </row>
     <row r="11" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J11" s="36">
+      <c r="J11" s="18">
         <v>6</v>
       </c>
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="44"/>
+      <c r="L11" s="34"/>
       <c r="N11" s="3">
         <v>8</v>
       </c>
-      <c r="O11" s="9"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="10"/>
+      <c r="R11" s="8"/>
       <c r="S11" s="6"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1437,7 +1480,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="9"/>
+      <c r="AB11" s="7"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
@@ -1445,27 +1488,27 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
-      <c r="AJ11" s="10"/>
+      <c r="AJ11" s="8"/>
       <c r="AK11" s="6"/>
       <c r="AL11" s="1"/>
-      <c r="AM11" s="10"/>
+      <c r="AM11" s="8"/>
       <c r="AN11" s="4"/>
     </row>
     <row r="12" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J12" s="36">
+      <c r="J12" s="18">
         <v>7</v>
       </c>
-      <c r="K12" s="41" t="s">
+      <c r="K12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="42"/>
+      <c r="L12" s="33"/>
       <c r="N12" s="5">
         <v>10</v>
       </c>
-      <c r="O12" s="9"/>
+      <c r="O12" s="7"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="10"/>
+      <c r="R12" s="8"/>
       <c r="S12" s="6"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1475,7 +1518,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="9"/>
+      <c r="AB12" s="7"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
@@ -1483,27 +1526,27 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
-      <c r="AJ12" s="10"/>
+      <c r="AJ12" s="8"/>
       <c r="AK12" s="6"/>
       <c r="AL12" s="1"/>
-      <c r="AM12" s="10"/>
+      <c r="AM12" s="8"/>
       <c r="AN12" s="4"/>
     </row>
     <row r="13" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J13" s="36">
+      <c r="J13" s="18">
         <v>8</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="K13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="44"/>
+      <c r="L13" s="34"/>
       <c r="N13" s="3">
         <v>15</v>
       </c>
-      <c r="O13" s="9"/>
+      <c r="O13" s="7"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="10"/>
+      <c r="R13" s="8"/>
       <c r="S13" s="6"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
@@ -1513,7 +1556,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="9"/>
+      <c r="AB13" s="7"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
@@ -1521,27 +1564,27 @@
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
-      <c r="AJ13" s="10"/>
+      <c r="AJ13" s="8"/>
       <c r="AK13" s="6"/>
       <c r="AL13" s="1"/>
-      <c r="AM13" s="10"/>
+      <c r="AM13" s="8"/>
       <c r="AN13" s="4"/>
     </row>
     <row r="14" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J14" s="36">
+      <c r="J14" s="18">
         <v>9</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="42"/>
+      <c r="L14" s="33"/>
       <c r="N14" s="5">
         <v>17</v>
       </c>
-      <c r="O14" s="9"/>
+      <c r="O14" s="7"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="10"/>
+      <c r="R14" s="8"/>
       <c r="S14" s="6"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -1551,7 +1594,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="9"/>
+      <c r="AB14" s="7"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
@@ -1559,27 +1602,27 @@
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
-      <c r="AJ14" s="10"/>
+      <c r="AJ14" s="8"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="1"/>
-      <c r="AM14" s="10"/>
+      <c r="AM14" s="8"/>
       <c r="AN14" s="4"/>
     </row>
     <row r="15" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J15" s="36">
+      <c r="J15" s="18">
         <v>10</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="41"/>
+      <c r="L15" s="32"/>
       <c r="N15" s="3">
         <v>22</v>
       </c>
-      <c r="O15" s="9"/>
+      <c r="O15" s="7"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="10"/>
+      <c r="R15" s="8"/>
       <c r="S15" s="6"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -1589,7 +1632,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="9"/>
+      <c r="AB15" s="7"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
@@ -1597,29 +1640,29 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
-      <c r="AJ15" s="10"/>
+      <c r="AJ15" s="8"/>
       <c r="AK15" s="6"/>
       <c r="AL15" s="1"/>
-      <c r="AM15" s="10"/>
+      <c r="AM15" s="8"/>
       <c r="AN15" s="4"/>
     </row>
     <row r="16" spans="7:40" x14ac:dyDescent="0.25">
-      <c r="J16" s="36">
+      <c r="J16" s="18">
         <v>11</v>
       </c>
-      <c r="K16" s="45" t="s">
+      <c r="K16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="22" t="s">
         <v>21</v>
       </c>
       <c r="N16" s="5">
         <v>24</v>
       </c>
-      <c r="O16" s="9"/>
+      <c r="O16" s="7"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="10"/>
+      <c r="R16" s="8"/>
       <c r="S16" s="6"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -1629,7 +1672,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="9"/>
+      <c r="AB16" s="7"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
@@ -1637,29 +1680,29 @@
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
-      <c r="AJ16" s="10"/>
+      <c r="AJ16" s="8"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="1"/>
-      <c r="AM16" s="10"/>
+      <c r="AM16" s="8"/>
       <c r="AN16" s="4"/>
     </row>
     <row r="17" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="J17" s="36">
+      <c r="J17" s="18">
         <v>12</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="K17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="53" t="s">
+      <c r="L17" s="27" t="s">
         <v>22</v>
       </c>
       <c r="N17" s="3">
         <v>29</v>
       </c>
-      <c r="O17" s="9"/>
+      <c r="O17" s="7"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="10"/>
+      <c r="R17" s="8"/>
       <c r="S17" s="6"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1669,7 +1712,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="9"/>
+      <c r="AB17" s="7"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
@@ -1677,27 +1720,27 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="10"/>
+      <c r="AJ17" s="8"/>
       <c r="AK17" s="6"/>
       <c r="AL17" s="1"/>
-      <c r="AM17" s="10"/>
+      <c r="AM17" s="8"/>
       <c r="AN17" s="4"/>
     </row>
     <row r="18" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="J18" s="36">
+      <c r="J18" s="18">
         <v>13</v>
       </c>
-      <c r="K18" s="47" t="s">
+      <c r="K18" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="47"/>
+      <c r="L18" s="35"/>
       <c r="N18" s="5">
         <v>1</v>
       </c>
-      <c r="O18" s="9"/>
+      <c r="O18" s="7"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="10"/>
+      <c r="R18" s="8"/>
       <c r="S18" s="6"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -1707,7 +1750,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="9"/>
+      <c r="AB18" s="7"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
@@ -1715,27 +1758,27 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="10"/>
+      <c r="AJ18" s="8"/>
       <c r="AK18" s="6"/>
       <c r="AL18" s="1"/>
-      <c r="AM18" s="10"/>
+      <c r="AM18" s="8"/>
       <c r="AN18" s="4"/>
     </row>
     <row r="19" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="J19" s="36">
+      <c r="J19" s="18">
         <v>14</v>
       </c>
-      <c r="K19" s="57" t="s">
+      <c r="K19" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="43"/>
+      <c r="L19" s="31"/>
       <c r="N19" s="3">
         <v>6</v>
       </c>
-      <c r="O19" s="9"/>
+      <c r="O19" s="7"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="10"/>
+      <c r="R19" s="8"/>
       <c r="S19" s="6"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -1745,7 +1788,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="9"/>
+      <c r="AB19" s="7"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
@@ -1753,25 +1796,25 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
-      <c r="AJ19" s="10"/>
+      <c r="AJ19" s="8"/>
       <c r="AK19" s="6"/>
       <c r="AL19" s="1"/>
-      <c r="AM19" s="10"/>
+      <c r="AM19" s="8"/>
       <c r="AN19" s="4"/>
     </row>
     <row r="20" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="J20" s="36">
+      <c r="J20" s="18">
         <v>15</v>
       </c>
-      <c r="K20" s="48"/>
-      <c r="L20" s="49"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="24"/>
       <c r="N20" s="5">
         <v>8</v>
       </c>
-      <c r="O20" s="9"/>
+      <c r="O20" s="7"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="10"/>
+      <c r="R20" s="8"/>
       <c r="S20" s="6"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -1781,7 +1824,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
-      <c r="AB20" s="9"/>
+      <c r="AB20" s="7"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
@@ -1789,22 +1832,22 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
-      <c r="AJ20" s="10"/>
+      <c r="AJ20" s="8"/>
       <c r="AK20" s="6"/>
       <c r="AL20" s="1"/>
-      <c r="AM20" s="10"/>
+      <c r="AM20" s="8"/>
       <c r="AN20" s="4"/>
     </row>
     <row r="21" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
       <c r="N21" s="3">
         <v>13</v>
       </c>
-      <c r="O21" s="9"/>
+      <c r="O21" s="7"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="10"/>
+      <c r="R21" s="8"/>
       <c r="S21" s="6"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1814,7 +1857,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
-      <c r="AB21" s="9"/>
+      <c r="AB21" s="7"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
@@ -1822,22 +1865,22 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
-      <c r="AJ21" s="10"/>
+      <c r="AJ21" s="8"/>
       <c r="AK21" s="6"/>
       <c r="AL21" s="1"/>
-      <c r="AM21" s="10"/>
+      <c r="AM21" s="8"/>
       <c r="AN21" s="4"/>
     </row>
     <row r="22" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
       <c r="N22" s="5">
         <v>15</v>
       </c>
-      <c r="O22" s="9"/>
+      <c r="O22" s="7"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="10"/>
+      <c r="R22" s="8"/>
       <c r="S22" s="6"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -1847,7 +1890,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
-      <c r="AB22" s="9"/>
+      <c r="AB22" s="7"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
@@ -1855,21 +1898,21 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
-      <c r="AJ22" s="10"/>
+      <c r="AJ22" s="8"/>
       <c r="AK22" s="6"/>
       <c r="AL22" s="1"/>
-      <c r="AM22" s="10"/>
+      <c r="AM22" s="8"/>
     </row>
     <row r="23" spans="10:40" x14ac:dyDescent="0.25">
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
       <c r="N23" s="3">
         <v>20</v>
       </c>
-      <c r="O23" s="9"/>
+      <c r="O23" s="7"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="10"/>
+      <c r="R23" s="8"/>
       <c r="S23" s="6"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -1879,7 +1922,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
-      <c r="AB23" s="9"/>
+      <c r="AB23" s="7"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
@@ -1887,19 +1930,19 @@
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
-      <c r="AJ23" s="10"/>
+      <c r="AJ23" s="8"/>
       <c r="AK23" s="6"/>
       <c r="AL23" s="1"/>
-      <c r="AM23" s="10"/>
+      <c r="AM23" s="8"/>
     </row>
     <row r="24" spans="10:40" x14ac:dyDescent="0.25">
       <c r="N24" s="5">
         <v>22</v>
       </c>
-      <c r="O24" s="9"/>
+      <c r="O24" s="7"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="10"/>
+      <c r="R24" s="8"/>
       <c r="S24" s="6"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -1909,7 +1952,7 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
-      <c r="AB24" s="9"/>
+      <c r="AB24" s="7"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
@@ -1917,19 +1960,19 @@
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
-      <c r="AJ24" s="10"/>
+      <c r="AJ24" s="8"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="1"/>
-      <c r="AM24" s="10"/>
+      <c r="AM24" s="8"/>
     </row>
     <row r="25" spans="10:40" x14ac:dyDescent="0.25">
       <c r="N25" s="3">
         <v>27</v>
       </c>
-      <c r="O25" s="9"/>
+      <c r="O25" s="7"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="10"/>
+      <c r="R25" s="8"/>
       <c r="S25" s="6"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -1939,7 +1982,7 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
-      <c r="AB25" s="9"/>
+      <c r="AB25" s="7"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
@@ -1947,19 +1990,19 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
-      <c r="AJ25" s="10"/>
+      <c r="AJ25" s="8"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="1"/>
-      <c r="AM25" s="10"/>
+      <c r="AM25" s="8"/>
     </row>
     <row r="26" spans="10:40" x14ac:dyDescent="0.25">
       <c r="N26" s="5">
         <v>29</v>
       </c>
-      <c r="O26" s="9"/>
+      <c r="O26" s="7"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="10"/>
+      <c r="R26" s="8"/>
       <c r="S26" s="6"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -1969,7 +2012,7 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
-      <c r="AB26" s="9"/>
+      <c r="AB26" s="7"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
@@ -1977,19 +2020,19 @@
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
-      <c r="AJ26" s="10"/>
+      <c r="AJ26" s="8"/>
       <c r="AK26" s="6"/>
       <c r="AL26" s="1"/>
-      <c r="AM26" s="10"/>
+      <c r="AM26" s="8"/>
     </row>
     <row r="27" spans="10:40" x14ac:dyDescent="0.25">
       <c r="N27" s="3">
         <v>3</v>
       </c>
-      <c r="O27" s="9"/>
+      <c r="O27" s="7"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="10"/>
+      <c r="R27" s="8"/>
       <c r="S27" s="6"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -1999,7 +2042,7 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
-      <c r="AB27" s="9"/>
+      <c r="AB27" s="7"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
@@ -2007,19 +2050,19 @@
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
-      <c r="AJ27" s="10"/>
+      <c r="AJ27" s="8"/>
       <c r="AK27" s="6"/>
       <c r="AL27" s="1"/>
-      <c r="AM27" s="10"/>
+      <c r="AM27" s="8"/>
     </row>
     <row r="28" spans="10:40" x14ac:dyDescent="0.25">
       <c r="N28" s="5">
         <v>5</v>
       </c>
-      <c r="O28" s="9"/>
+      <c r="O28" s="7"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="10"/>
+      <c r="R28" s="8"/>
       <c r="S28" s="6"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -2029,7 +2072,7 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
-      <c r="AB28" s="9"/>
+      <c r="AB28" s="7"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
@@ -2037,61 +2080,44 @@
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
-      <c r="AJ28" s="10"/>
+      <c r="AJ28" s="8"/>
       <c r="AK28" s="6"/>
       <c r="AL28" s="1"/>
-      <c r="AM28" s="10"/>
+      <c r="AM28" s="8"/>
     </row>
     <row r="29" spans="10:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N29" s="3">
         <v>10</v>
       </c>
-      <c r="O29" s="11"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12"/>
-      <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
-      <c r="AH29" s="12"/>
-      <c r="AI29" s="12"/>
-      <c r="AJ29" s="13"/>
-      <c r="AK29" s="24"/>
-      <c r="AL29" s="12"/>
-      <c r="AM29" s="13"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="10"/>
+      <c r="AD29" s="10"/>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="10"/>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="17"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
+  <mergeCells count="29">
+    <mergeCell ref="O1:AM1"/>
     <mergeCell ref="AK4:AM4"/>
     <mergeCell ref="S3:AA3"/>
     <mergeCell ref="O3:R3"/>
@@ -2102,6 +2128,24 @@
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>